<commit_message>
Consertando o caminho do Docker, adicionado o primeiro usuário, e exportando para o Excel
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>JULIA</t>
+          <t>Matheus Schmitz Glanzmann</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>JULIA</t>
+          <t>schmitzmatheus321@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>50505050</t>
+          <t>40630910</t>
         </is>
       </c>
     </row>

</xml_diff>